<commit_message>
chains created, counting stats now
</commit_message>
<xml_diff>
--- a/data/nouns/pairwise_stats.xlsx
+++ b/data/nouns/pairwise_stats.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="pairwise_stats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1157,10 +1157,10 @@
   <dimension ref="A1:DC104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CN83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DB104" sqref="DB104"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>